<commit_message>
update missing stories, add unknow cards
</commit_message>
<xml_diff>
--- a/src/data/stories.xlsx
+++ b/src/data/stories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsbch\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsbch\Music\testproject\onmyojigame-paper-role-main\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB727A09-198A-4C9F-8894-E176F0160A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8621850B-99FE-4BD2-BFA1-CCC62FDBB866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-9975" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="418">
   <si>
     <t>id</t>
   </si>
@@ -1159,9 +1159,6 @@
     <t>["Oitsukigami","Bukkuman","Ushi no Toki","Ibaraki Doji","Kiyohime"]</t>
   </si>
   <si>
-    <t>[""]</t>
-  </si>
-  <si>
     <t>["Hakuzosu","Kawazaru"]</t>
   </si>
   <si>
@@ -1256,13 +1253,34 @@
   </si>
   <si>
     <t>["Kotodama","Kagura"]</t>
+  </si>
+  <si>
+    <t>["Ungaikyo","Zen Ungaikyo"]</t>
+  </si>
+  <si>
+    <t>["Yamalord Enma","Hangan","Kuro Mujou","Shiro Mujou","Mouba"]</t>
+  </si>
+  <si>
+    <t>["Heartseeker Momiji","Seimei"]</t>
+  </si>
+  <si>
+    <t>["Fukengaku","Momo","Sakura"]</t>
+  </si>
+  <si>
+    <t>["Shokurei","Mishige","Amezaiku"]</t>
+  </si>
+  <si>
+    <t>["Shokurei","Mishige"]</t>
+  </si>
+  <si>
+    <t>["Inaba Kaguya","Mannendake","Ootengu","Hiromasa","unknow"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1285,9 +1303,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFADBAC7"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1310,7 +1340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1327,11 +1357,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color auto="1"/>
+      </font>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1370,7 +1414,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B3FAA137-9282-4B98-8FF5-6233E764B041}" name="Table1" displayName="Table1" ref="A1:E139" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B3FAA137-9282-4B98-8FF5-6233E764B041}" name="Table1" displayName="Table1" ref="A1:E139" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:E139" xr:uid="{B3FAA137-9282-4B98-8FF5-6233E764B041}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1379,11 +1423,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{320C8A9B-17E2-4662-A458-EB196C9158CD}" name="id" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{320C8A9B-17E2-4662-A458-EB196C9158CD}" name="id" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{14D29A2D-1724-47CA-A383-648B6704CF04}" name="name"/>
-    <tableColumn id="3" xr3:uid="{24BA9719-40EA-42E8-8BD9-57F296097FF8}" name="point" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{32756F44-F754-4E66-B169-22537D96923C}" name="text" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{26501923-DF31-4CD2-AB6B-CD7681D43798}" name="cards"/>
+    <tableColumn id="3" xr3:uid="{24BA9719-40EA-42E8-8BD9-57F296097FF8}" name="point" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{32756F44-F754-4E66-B169-22537D96923C}" name="text" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{26501923-DF31-4CD2-AB6B-CD7681D43798}" name="cards" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1713,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="H140" sqref="H140"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1723,7 +1767,7 @@
     <col min="2" max="2" width="21.625" customWidth="1"/>
     <col min="3" max="3" width="9" style="2"/>
     <col min="4" max="4" width="85.25" customWidth="1"/>
-    <col min="5" max="5" width="52.25" customWidth="1"/>
+    <col min="5" max="5" width="69.375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1739,7 +1783,7 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3440,7 +3484,7 @@
         <v>203</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>379</v>
+        <v>416</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3457,7 +3501,7 @@
         <v>205</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>379</v>
+        <v>415</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3474,7 +3518,7 @@
         <v>207</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3491,7 +3535,7 @@
         <v>208</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3508,7 +3552,7 @@
         <v>211</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3525,7 +3569,7 @@
         <v>213</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3542,7 +3586,7 @@
         <v>215</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>379</v>
+        <v>417</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3559,7 +3603,7 @@
         <v>217</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3576,7 +3620,7 @@
         <v>219</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3593,7 +3637,7 @@
         <v>221</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3610,7 +3654,7 @@
         <v>223</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>379</v>
+        <v>414</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3627,7 +3671,7 @@
         <v>225</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3644,7 +3688,7 @@
         <v>227</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3661,7 +3705,7 @@
         <v>229</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3678,7 +3722,7 @@
         <v>232</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3695,7 +3739,7 @@
         <v>233</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3712,7 +3756,7 @@
         <v>235</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3729,7 +3773,7 @@
         <v>237</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3746,7 +3790,7 @@
         <v>239</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3763,7 +3807,7 @@
         <v>241</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3780,7 +3824,7 @@
         <v>244</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3797,7 +3841,7 @@
         <v>245</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3814,7 +3858,7 @@
         <v>247</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>379</v>
+        <v>412</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3831,7 +3875,7 @@
         <v>249</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>379</v>
+        <v>413</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3848,7 +3892,7 @@
         <v>251</v>
       </c>
       <c r="E125" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3865,7 +3909,7 @@
         <v>253</v>
       </c>
       <c r="E126" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3882,7 +3926,7 @@
         <v>256</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3899,7 +3943,7 @@
         <v>257</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3916,7 +3960,7 @@
         <v>259</v>
       </c>
       <c r="E129" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3933,7 +3977,7 @@
         <v>261</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3950,7 +3994,7 @@
         <v>263</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3967,7 +4011,7 @@
         <v>265</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3984,7 +4028,7 @@
         <v>268</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4001,7 +4045,7 @@
         <v>269</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4018,7 +4062,7 @@
         <v>272</v>
       </c>
       <c r="E135" s="5" t="s">
-        <v>379</v>
+        <v>411</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4035,7 +4079,7 @@
         <v>273</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4052,7 +4096,7 @@
         <v>276</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4069,7 +4113,7 @@
         <v>277</v>
       </c>
       <c r="E138" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4086,7 +4130,7 @@
         <v>279</v>
       </c>
       <c r="E139" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>